<commit_message>
Fix DB logic, ratings, and handlers
</commit_message>
<xml_diff>
--- a/menejerlar_reytingi.xlsx
+++ b/menejerlar_reytingi.xlsx
@@ -463,10 +463,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4.78</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>4.4</v>
       </c>
       <c r="D3" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>

</xml_diff>